<commit_message>
Add booth column in club import file
</commit_message>
<xml_diff>
--- a/resources/sample/club_import_sample.xlsx
+++ b/resources/sample/club_import_sample.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CheckIn2017\resources\sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CheckIn\resources\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4C96FC67-3457-4D9A-B540-68C9FC4EE621}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>社團名稱</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -75,6 +76,14 @@
   </si>
   <si>
     <t>攤位負責人5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>攤位編號</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>D15</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -162,17 +171,7 @@
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="合計" xfId="1" builtinId="25"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -503,21 +502,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.25" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.25" customWidth="1"/>
+    <col min="5" max="9" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -528,22 +528,25 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="17.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -554,18 +557,21 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:H1048576">
+  <conditionalFormatting sqref="E1:I1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update club import format
</commit_message>
<xml_diff>
--- a/resources/sample/club_import_sample.xlsx
+++ b/resources/sample/club_import_sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CheckIn\resources\sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\CheckIn\resources\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4C96FC67-3457-4D9A-B540-68C9FC4EE621}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE4F1ED-579F-4066-A557-84CEE6AA8E42}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -59,39 +59,36 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>攤位負責人1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>攤位負責人2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>攤位負責人3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>攤位負責人4</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>攤位負責人5</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>攤位編號</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>D15</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>社長</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>工作人員1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>工作人員2</t>
+  </si>
+  <si>
+    <t>工作人員3</t>
+  </si>
+  <si>
+    <t>工作人員4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -115,6 +112,14 @@
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
     </font>
   </fonts>
   <fills count="2">
@@ -153,7 +158,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -164,6 +169,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -506,7 +514,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -528,22 +536,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17.25" thickTop="1" x14ac:dyDescent="0.25">
@@ -557,7 +565,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Increase staff limit from 4+1 to 6+1
</commit_message>
<xml_diff>
--- a/resources/sample/club_import_sample.xlsx
+++ b/resources/sample/club_import_sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\CheckIn\resources\sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CheckIn\resources\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE4F1ED-579F-4066-A557-84CEE6AA8E42}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C659335A-50AA-45BF-81CA-D8DE0BB17AA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>社團名稱</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -82,6 +82,14 @@
   </si>
   <si>
     <t>工作人員4</t>
+  </si>
+  <si>
+    <t>工作人員5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>工作人員6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -510,11 +518,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -522,10 +530,10 @@
     <col min="1" max="1" width="10.25" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.25" customWidth="1"/>
-    <col min="5" max="9" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="11" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -553,8 +561,14 @@
       <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="17.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="17.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -579,7 +593,7 @@
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:I1048576">
+  <conditionalFormatting sqref="E1:K1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>